<commit_message>
updated to new format
</commit_message>
<xml_diff>
--- a/locations_test.xlsx
+++ b/locations_test.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="365">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="366">
   <si>
     <t xml:space="preserve">#</t>
   </si>
@@ -345,6 +345,9 @@
   </si>
   <si>
     <t xml:space="preserve">41.8911897,-87.6262266</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7 Massacre</t>
   </si>
   <si>
     <t xml:space="preserve">1929-02-14 10:30:00</t>
@@ -1126,7 +1129,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1148,12 +1151,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -1239,7 +1236,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1334,9 +1331,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>304560</xdr:colOff>
+      <xdr:colOff>304200</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>25200</xdr:rowOff>
+      <xdr:rowOff>24840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1350,7 +1347,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="190440"/>
-          <a:ext cx="304560" cy="304560"/>
+          <a:ext cx="304200" cy="304200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1371,9 +1368,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>304560</xdr:colOff>
+      <xdr:colOff>304200</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>25200</xdr:rowOff>
+      <xdr:rowOff>24840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1387,7 +1384,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="469800"/>
-          <a:ext cx="304560" cy="304560"/>
+          <a:ext cx="304200" cy="304200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1408,9 +1405,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>304560</xdr:colOff>
+      <xdr:colOff>304200</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>12600</xdr:rowOff>
+      <xdr:rowOff>12240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1424,7 +1421,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="749160"/>
-          <a:ext cx="304560" cy="304560"/>
+          <a:ext cx="304200" cy="304200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1445,9 +1442,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>304560</xdr:colOff>
+      <xdr:colOff>304200</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>12240</xdr:rowOff>
+      <xdr:rowOff>11880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1461,7 +1458,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="1041120"/>
-          <a:ext cx="304560" cy="304560"/>
+          <a:ext cx="304200" cy="304200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1482,9 +1479,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>44640</xdr:colOff>
+      <xdr:colOff>44280</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>25200</xdr:rowOff>
+      <xdr:rowOff>24840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1498,7 +1495,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="1333440"/>
-          <a:ext cx="609120" cy="609120"/>
+          <a:ext cx="608760" cy="608760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1519,9 +1516,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>304560</xdr:colOff>
+      <xdr:colOff>304200</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>304560</xdr:rowOff>
+      <xdr:rowOff>304200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1535,7 +1532,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="1917360"/>
-          <a:ext cx="304560" cy="304560"/>
+          <a:ext cx="304200" cy="304200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1556,9 +1553,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>304560</xdr:colOff>
+      <xdr:colOff>304200</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>25200</xdr:rowOff>
+      <xdr:rowOff>24840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1572,7 +1569,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="2222280"/>
-          <a:ext cx="304560" cy="304560"/>
+          <a:ext cx="304200" cy="304200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1593,9 +1590,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>304560</xdr:colOff>
+      <xdr:colOff>304200</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>25200</xdr:rowOff>
+      <xdr:rowOff>24840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1609,7 +1606,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="2501640"/>
-          <a:ext cx="304560" cy="304560"/>
+          <a:ext cx="304200" cy="304200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1630,9 +1627,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>304560</xdr:colOff>
+      <xdr:colOff>304200</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>25200</xdr:rowOff>
+      <xdr:rowOff>24840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1646,7 +1643,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="2781000"/>
-          <a:ext cx="304560" cy="304560"/>
+          <a:ext cx="304200" cy="304200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1667,9 +1664,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>304560</xdr:colOff>
+      <xdr:colOff>304200</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>12240</xdr:rowOff>
+      <xdr:rowOff>11880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1683,7 +1680,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="3060360"/>
-          <a:ext cx="304560" cy="304560"/>
+          <a:ext cx="304200" cy="304200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1704,9 +1701,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>304560</xdr:colOff>
+      <xdr:colOff>304200</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>12600</xdr:rowOff>
+      <xdr:rowOff>12240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1720,7 +1717,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="3352680"/>
-          <a:ext cx="304560" cy="304560"/>
+          <a:ext cx="304200" cy="304200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1741,9 +1738,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>304560</xdr:colOff>
+      <xdr:colOff>304200</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>304560</xdr:rowOff>
+      <xdr:rowOff>304200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1757,7 +1754,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="3644640"/>
-          <a:ext cx="304560" cy="304560"/>
+          <a:ext cx="304200" cy="304200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1778,9 +1775,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>304560</xdr:colOff>
+      <xdr:colOff>304200</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>304560</xdr:rowOff>
+      <xdr:rowOff>304200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1794,7 +1791,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="3962160"/>
-          <a:ext cx="304560" cy="304560"/>
+          <a:ext cx="304200" cy="304200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1815,9 +1812,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>304560</xdr:colOff>
+      <xdr:colOff>304200</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>12240</xdr:rowOff>
+      <xdr:rowOff>11880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1831,7 +1828,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="4279680"/>
-          <a:ext cx="304560" cy="304560"/>
+          <a:ext cx="304200" cy="304200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1852,9 +1849,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>44640</xdr:colOff>
+      <xdr:colOff>44280</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>126360</xdr:rowOff>
+      <xdr:rowOff>126000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1868,7 +1865,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="4647960"/>
-          <a:ext cx="609120" cy="609120"/>
+          <a:ext cx="608760" cy="608760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1889,9 +1886,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>44640</xdr:colOff>
+      <xdr:colOff>44280</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>126720</xdr:rowOff>
+      <xdr:rowOff>126360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1905,7 +1902,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="5130720"/>
-          <a:ext cx="609120" cy="609120"/>
+          <a:ext cx="608760" cy="608760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1926,9 +1923,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>44640</xdr:colOff>
+      <xdr:colOff>44280</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>126360</xdr:rowOff>
+      <xdr:rowOff>126000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1942,7 +1939,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="5613120"/>
-          <a:ext cx="609120" cy="609120"/>
+          <a:ext cx="608760" cy="608760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1963,9 +1960,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>44640</xdr:colOff>
+      <xdr:colOff>44280</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>126720</xdr:rowOff>
+      <xdr:rowOff>126360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1979,7 +1976,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="6095880"/>
-          <a:ext cx="609120" cy="609120"/>
+          <a:ext cx="608760" cy="608760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2000,9 +1997,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>44640</xdr:colOff>
+      <xdr:colOff>44280</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>50040</xdr:rowOff>
+      <xdr:rowOff>49680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2016,7 +2013,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="6578280"/>
-          <a:ext cx="609120" cy="609120"/>
+          <a:ext cx="608760" cy="608760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2037,9 +2034,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>44640</xdr:colOff>
+      <xdr:colOff>44280</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>151920</xdr:rowOff>
+      <xdr:rowOff>151560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2053,7 +2050,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="7137360"/>
-          <a:ext cx="609120" cy="609120"/>
+          <a:ext cx="608760" cy="608760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2083,14 +2080,14 @@
       <selection pane="bottomRight" activeCell="E11" activeCellId="0" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="44.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="0" width="10"/>
@@ -2110,8 +2107,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="27" style="0" width="10.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="22.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="20.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="0" width="30.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="20.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="0" width="30.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="33" style="0" width="19.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="0" width="10"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="0" width="14.01"/>
@@ -2122,11 +2119,11 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="0" width="18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="0" width="10"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="0" width="25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="0" width="20.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="0" width="20.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="45" min="45" style="0" width="9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="46" style="0" width="10"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="47" style="0" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="0" width="15.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="0" width="15.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="49" style="0" width="6.01"/>
   </cols>
   <sheetData>
@@ -2686,26 +2683,26 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
-        <v>7</v>
+      <c r="A7" s="0" t="s">
+        <v>108</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="L7" s="0" t="s">
         <v>55</v>
@@ -2714,16 +2711,16 @@
         <v>56</v>
       </c>
       <c r="Q7" s="3" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="R7" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="S7" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="T7" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="U7" s="0" t="s">
         <v>62</v>
@@ -2735,19 +2732,19 @@
         <v>64</v>
       </c>
       <c r="Y7" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="Z7" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="AF7" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="AG7" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="AH7" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="AR7" s="5" t="n">
         <v>10638.4375</v>
@@ -2762,7 +2759,7 @@
         <v>56</v>
       </c>
       <c r="AV7" s="5" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="AW7" s="0" t="n">
         <v>7</v>
@@ -2773,34 +2770,34 @@
         <v>8</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="M8" s="0" t="s">
         <v>56</v>
       </c>
       <c r="P8" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="Q8" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="S8" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="T8" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="U8" s="0" t="s">
         <v>62</v>
@@ -2809,31 +2806,31 @@
         <v>63</v>
       </c>
       <c r="W8" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="X8" s="0" t="s">
         <v>64</v>
       </c>
       <c r="Y8" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="Z8" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="AF8" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="AG8" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="AH8" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="AR8" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="AT8" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="AU8" s="0" t="s">
         <v>56</v>
@@ -2847,22 +2844,22 @@
         <v>9</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="M9" s="0" t="s">
         <v>56</v>
       </c>
       <c r="P9" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="T9" s="0" t="s">
         <v>61</v>
@@ -2874,43 +2871,43 @@
         <v>63</v>
       </c>
       <c r="W9" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="X9" s="0" t="s">
         <v>64</v>
       </c>
       <c r="Y9" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="Z9" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="AB9" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="AE9" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="AF9" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="AG9" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="AH9" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="AK9" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="AM9" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="AR9" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="AT9" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="AU9" s="0" t="s">
         <v>56</v>
@@ -2924,31 +2921,31 @@
         <v>10</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="L10" s="0" t="s">
         <v>55</v>
       </c>
       <c r="M10" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="P10" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="Q10" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="T10" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="U10" s="0" t="s">
         <v>62</v>
@@ -2957,46 +2954,46 @@
         <v>63</v>
       </c>
       <c r="W10" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="X10" s="0" t="s">
         <v>64</v>
       </c>
       <c r="Y10" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="Z10" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="AB10" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="AC10" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="AD10" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="AE10" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AF10" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="AG10" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="AH10" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="AK10" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="AR10" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="AT10" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="AU10" s="0" t="s">
         <v>56</v>
@@ -3010,13 +3007,13 @@
         <v>11</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="I11" s="0" t="s">
         <v>54</v>
@@ -3025,37 +3022,37 @@
         <v>56</v>
       </c>
       <c r="P11" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="T11" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="V11" s="0" t="s">
         <v>63</v>
       </c>
       <c r="W11" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="X11" s="0" t="s">
         <v>64</v>
       </c>
       <c r="Y11" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="Z11" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="AF11" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="AG11" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="AH11" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="AR11" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="AT11" s="0" t="s">
         <v>54</v>
@@ -3072,67 +3069,67 @@
         <v>12</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="M12" s="0" t="s">
         <v>56</v>
       </c>
       <c r="P12" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="R12" s="0" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="S12" s="0" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="T12" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="V12" s="0" t="s">
         <v>63</v>
       </c>
       <c r="W12" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="X12" s="0" t="s">
         <v>64</v>
       </c>
       <c r="Y12" s="0" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="Z12" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="AB12" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="AE12" s="0" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="AF12" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="AG12" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="AH12" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="AR12" s="0" t="s">
         <v>177</v>
       </c>
-      <c r="AR12" s="0" t="s">
-        <v>176</v>
-      </c>
       <c r="AT12" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="AU12" s="0" t="s">
         <v>56</v>
@@ -3146,61 +3143,61 @@
         <v>13</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="M13" s="0" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="P13" s="0" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="Q13" s="0" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="U13" s="0" t="s">
         <v>62</v>
       </c>
       <c r="V13" s="0" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="X13" s="0" t="s">
         <v>64</v>
       </c>
       <c r="Y13" s="0" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="AE13" s="0" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="AF13" s="0" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="AG13" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="AH13" s="0" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="AK13" s="0" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="AQ13" s="0" t="n">
         <v>230</v>
       </c>
       <c r="AR13" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AT13" s="0" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="AU13" s="0" t="s">
         <v>56</v>
@@ -3214,58 +3211,58 @@
         <v>14</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="M14" s="0" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="P14" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="Q14" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="T14" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="V14" s="0" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="X14" s="0" t="s">
         <v>64</v>
       </c>
       <c r="Y14" s="0" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="AE14" s="0" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AF14" s="0" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="AG14" s="0" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="AH14" s="0" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="AQ14" s="0" t="n">
         <v>257</v>
       </c>
       <c r="AR14" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="AT14" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="AU14" s="0" t="s">
         <v>56</v>
@@ -3279,25 +3276,25 @@
         <v>15</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="M15" s="0" t="s">
         <v>56</v>
       </c>
       <c r="P15" s="0" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="T15" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="U15" s="0" t="s">
         <v>62</v>
@@ -3306,31 +3303,31 @@
         <v>63</v>
       </c>
       <c r="W15" s="0" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="X15" s="0" t="s">
         <v>64</v>
       </c>
       <c r="Y15" s="0" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="Z15" s="0" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="AF15" s="0" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="AG15" s="0" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="AH15" s="0" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="AR15" s="0" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="AT15" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AU15" s="0" t="s">
         <v>56</v>
@@ -3344,31 +3341,31 @@
         <v>16</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="M16" s="0" t="s">
         <v>56</v>
       </c>
       <c r="P16" s="0" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="T16" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="U16" s="0" t="s">
         <v>62</v>
@@ -3377,28 +3374,28 @@
         <v>63</v>
       </c>
       <c r="W16" s="0" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="X16" s="0" t="s">
         <v>64</v>
       </c>
       <c r="Y16" s="0" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="AF16" s="0" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="AG16" s="0" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="AH16" s="0" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="AR16" s="0" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="AT16" s="0" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="AU16" s="0" t="s">
         <v>56</v>
@@ -3412,16 +3409,16 @@
         <v>17</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="I17" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="L17" s="0" t="s">
         <v>55</v>
@@ -3430,7 +3427,7 @@
         <v>56</v>
       </c>
       <c r="P17" s="0" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="T17" s="0" t="s">
         <v>61</v>
@@ -3442,31 +3439,31 @@
         <v>63</v>
       </c>
       <c r="W17" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="X17" s="0" t="s">
         <v>64</v>
       </c>
       <c r="Y17" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="Z17" s="0" t="s">
+        <v>225</v>
+      </c>
+      <c r="AF17" s="0" t="s">
+        <v>226</v>
+      </c>
+      <c r="AG17" s="0" t="s">
         <v>224</v>
       </c>
-      <c r="AF17" s="0" t="s">
-        <v>225</v>
-      </c>
-      <c r="AG17" s="0" t="s">
-        <v>223</v>
-      </c>
       <c r="AH17" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="AR17" s="0" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="AT17" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AU17" s="0" t="s">
         <v>56</v>
@@ -3480,28 +3477,28 @@
         <v>18</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="I18" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="M18" s="0" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="P18" s="0" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="Q18" s="0" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="S18" s="0" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="T18" s="0" t="s">
         <v>61</v>
@@ -3510,37 +3507,37 @@
         <v>62</v>
       </c>
       <c r="V18" s="0" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="X18" s="0" t="s">
         <v>64</v>
       </c>
       <c r="Y18" s="0" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="AE18" s="0" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="AF18" s="0" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="AG18" s="0" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="AH18" s="0" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="AK18" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="AQ18" s="0" t="n">
         <v>17</v>
       </c>
       <c r="AR18" s="0" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="AT18" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="AU18" s="0" t="s">
         <v>56</v>
@@ -3554,61 +3551,61 @@
         <v>19</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="I19" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="M19" s="0" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="P19" s="0" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="Q19" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="U19" s="0" t="s">
         <v>62</v>
       </c>
       <c r="V19" s="0" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="X19" s="0" t="s">
         <v>64</v>
       </c>
       <c r="Y19" s="0" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="AE19" s="0" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="AF19" s="0" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AG19" s="0" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="AH19" s="0" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="AK19" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="AQ19" s="0" t="n">
         <v>18</v>
       </c>
       <c r="AR19" s="0" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="AT19" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="AU19" s="0" t="s">
         <v>56</v>
@@ -3622,28 +3619,28 @@
         <v>20</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="I20" s="0" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="M20" s="0" t="s">
         <v>56</v>
       </c>
       <c r="P20" s="0" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="Q20" s="0" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="T20" s="0" t="s">
         <v>61</v>
@@ -3655,34 +3652,34 @@
         <v>63</v>
       </c>
       <c r="W20" s="0" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="X20" s="0" t="s">
         <v>64</v>
       </c>
       <c r="Y20" s="0" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="Z20" s="0" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AC20" s="0" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AF20" s="0" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AG20" s="0" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AH20" s="0" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AR20" s="0" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AT20" s="0" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AU20" s="0" t="s">
         <v>56</v>
@@ -3696,22 +3693,22 @@
         <v>21</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="I21" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="M21" s="0" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="P21" s="0" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="U21" s="0" t="s">
         <v>62</v>
@@ -3720,31 +3717,31 @@
         <v>64</v>
       </c>
       <c r="Y21" s="0" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AE21" s="0" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AF21" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AG21" s="0" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AH21" s="0" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AK21" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="AQ21" s="0" t="n">
         <v>109</v>
       </c>
       <c r="AR21" s="0" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AT21" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="AU21" s="0" t="s">
         <v>56</v>
@@ -3758,31 +3755,31 @@
         <v>22</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="I22" s="0" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="M22" s="0" t="s">
         <v>56</v>
       </c>
       <c r="P22" s="0" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="Q22" s="0" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="T22" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="U22" s="0" t="s">
         <v>62</v>
@@ -3791,28 +3788,28 @@
         <v>63</v>
       </c>
       <c r="W22" s="0" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="X22" s="0" t="s">
         <v>64</v>
       </c>
       <c r="Y22" s="0" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="Z22" s="0" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="AF22" s="0" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="AG22" s="0" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="AH22" s="0" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="AT22" s="0" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="AU22" s="0" t="s">
         <v>56</v>
@@ -3829,7 +3826,7 @@
         <v>56</v>
       </c>
       <c r="P23" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="U23" s="0" t="s">
         <v>62</v>
@@ -3849,28 +3846,28 @@
         <v>24</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="I24" s="0" t="s">
         <v>54</v>
       </c>
       <c r="L24" s="0" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="M24" s="0" t="s">
         <v>56</v>
       </c>
       <c r="P24" s="0" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="Q24" s="0" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="T24" s="0" t="s">
         <v>61</v>
@@ -3882,28 +3879,28 @@
         <v>63</v>
       </c>
       <c r="W24" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="X24" s="0" t="s">
         <v>64</v>
       </c>
       <c r="Y24" s="0" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="Z24" s="0" t="s">
+        <v>280</v>
+      </c>
+      <c r="AF24" s="0" t="s">
+        <v>285</v>
+      </c>
+      <c r="AG24" s="0" t="s">
+        <v>278</v>
+      </c>
+      <c r="AH24" s="0" t="s">
         <v>279</v>
       </c>
-      <c r="AF24" s="0" t="s">
-        <v>284</v>
-      </c>
-      <c r="AG24" s="0" t="s">
-        <v>277</v>
-      </c>
-      <c r="AH24" s="0" t="s">
-        <v>278</v>
-      </c>
       <c r="AT24" s="0" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="AU24" s="0" t="s">
         <v>56</v>
@@ -3917,28 +3914,28 @@
         <v>25</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="I25" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="M25" s="0" t="s">
         <v>56</v>
       </c>
       <c r="P25" s="0" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="Q25" s="0" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="T25" s="0" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="U25" s="0" t="s">
         <v>62</v>
@@ -3947,28 +3944,28 @@
         <v>63</v>
       </c>
       <c r="W25" s="0" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="X25" s="0" t="s">
         <v>64</v>
       </c>
       <c r="Y25" s="0" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="Z25" s="0" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="AF25" s="0" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="AG25" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="AH25" s="0" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="AT25" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AU25" s="0" t="s">
         <v>56</v>
@@ -3982,25 +3979,25 @@
         <v>26</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="I26" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="L26" s="0" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="M26" s="0" t="s">
         <v>56</v>
       </c>
       <c r="P26" s="0" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="Q26" s="0" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="T26" s="0" t="s">
         <v>61</v>
@@ -4012,28 +4009,28 @@
         <v>63</v>
       </c>
       <c r="W26" s="0" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="X26" s="0" t="s">
         <v>64</v>
       </c>
       <c r="Y26" s="0" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="Z26" s="0" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="AF26" s="0" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="AG26" s="0" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="AH26" s="0" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="AT26" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="AU26" s="0" t="s">
         <v>56</v>
@@ -4047,34 +4044,34 @@
         <v>27</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="H27" s="0" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="I27" s="0" t="s">
+        <v>307</v>
+      </c>
+      <c r="L27" s="0" t="s">
+        <v>281</v>
+      </c>
+      <c r="M27" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="P27" s="0" t="s">
+        <v>308</v>
+      </c>
+      <c r="Q27" s="0" t="s">
         <v>306</v>
       </c>
-      <c r="L27" s="0" t="s">
-        <v>280</v>
-      </c>
-      <c r="M27" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="P27" s="0" t="s">
-        <v>307</v>
-      </c>
-      <c r="Q27" s="0" t="s">
-        <v>305</v>
-      </c>
       <c r="T27" s="0" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="U27" s="0" t="s">
         <v>62</v>
@@ -4083,28 +4080,28 @@
         <v>63</v>
       </c>
       <c r="W27" s="0" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="X27" s="0" t="s">
         <v>64</v>
       </c>
       <c r="Y27" s="0" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="Z27" s="0" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="AF27" s="0" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="AG27" s="0" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="AH27" s="0" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="AT27" s="0" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="AU27" s="0" t="s">
         <v>56</v>
@@ -4118,13 +4115,13 @@
         <v>28</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="L28" s="0" t="s">
         <v>55</v>
@@ -4133,13 +4130,13 @@
         <v>56</v>
       </c>
       <c r="P28" s="0" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="Q28" s="0" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="T28" s="0" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="U28" s="0" t="s">
         <v>62</v>
@@ -4148,25 +4145,25 @@
         <v>63</v>
       </c>
       <c r="W28" s="0" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="X28" s="0" t="s">
         <v>64</v>
       </c>
       <c r="Y28" s="0" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="Z28" s="0" t="s">
+        <v>317</v>
+      </c>
+      <c r="AF28" s="0" t="s">
+        <v>322</v>
+      </c>
+      <c r="AG28" s="0" t="s">
+        <v>315</v>
+      </c>
+      <c r="AH28" s="0" t="s">
         <v>316</v>
-      </c>
-      <c r="AF28" s="0" t="s">
-        <v>321</v>
-      </c>
-      <c r="AG28" s="0" t="s">
-        <v>314</v>
-      </c>
-      <c r="AH28" s="0" t="s">
-        <v>315</v>
       </c>
       <c r="AT28" s="0" t="s">
         <v>54</v>
@@ -4183,19 +4180,19 @@
         <v>29</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="M29" s="0" t="s">
         <v>56</v>
       </c>
       <c r="P29" s="0" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="S29" s="0" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="T29" s="0" t="s">
         <v>61</v>
@@ -4207,25 +4204,25 @@
         <v>63</v>
       </c>
       <c r="W29" s="0" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="X29" s="0" t="s">
         <v>64</v>
       </c>
       <c r="Y29" s="0" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="AF29" s="0" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="AG29" s="0" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="AH29" s="0" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="AT29" s="0" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="AU29" s="0" t="s">
         <v>56</v>
@@ -4239,43 +4236,43 @@
         <v>30</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="M30" s="0" t="s">
         <v>56</v>
       </c>
       <c r="P30" s="0" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="R30" s="0" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="T30" s="0" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="V30" s="0" t="s">
         <v>63</v>
       </c>
       <c r="W30" s="0" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="X30" s="0" t="s">
         <v>64</v>
       </c>
       <c r="Y30" s="0" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="AF30" s="0" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="AG30" s="0" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="AH30" s="0" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="AT30" s="0" t="s">
         <v>99</v>
@@ -4313,71 +4310,71 @@
       <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="28.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="28.98"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>45</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="22" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="22" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="23" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="23" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="40" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="8" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="22" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4390,10 +4387,10 @@
     </row>
     <row r="10" customFormat="false" ht="22" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="22" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4401,114 +4398,114 @@
         <v>54</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="23" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="23" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B13" s="0" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="23" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="18" customFormat="false" ht="38" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="38" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B19" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="38" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B20" s="0" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="38" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B21" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="38" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B22" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B25" s="0" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="0" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
     </row>
   </sheetData>

</xml_diff>